<commit_message>
From bjo-sea01 fix redundant 2023-12-01.003846
</commit_message>
<xml_diff>
--- a/config/config/data-structure.SEA01.xlsx
+++ b/config/config/data-structure.SEA01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/Documents/docker/data/client/ysh/client/bjo-sea01/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1718C554-4655-A444-8366-5482E465F96D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3CF358-A5C4-F541-A137-D26449287D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="6160" windowWidth="28360" windowHeight="17620" activeTab="6" xr2:uid="{A25778A6-52F4-354B-B7EA-075EA69C9E88}"/>
+    <workbookView xWindow="2040" yWindow="6160" windowWidth="28360" windowHeight="17620" firstSheet="33" activeTab="43" xr2:uid="{A25778A6-52F4-354B-B7EA-075EA69C9E88}"/>
   </bookViews>
   <sheets>
     <sheet name="FSY-01-UNLOADING" sheetId="1" r:id="rId1"/>
@@ -18,20 +18,20 @@
     <sheet name="FSY-03-RECEIVING" sheetId="3" r:id="rId3"/>
     <sheet name="FSY-04-FREEZING" sheetId="4" r:id="rId4"/>
     <sheet name="FSY-05-STORING" sheetId="5" r:id="rId5"/>
-    <sheet name="FISH_CARD_GENERATOR" sheetId="27" r:id="rId6"/>
-    <sheet name="FISH_LABEL_GENERATOR" sheetId="34" r:id="rId7"/>
-    <sheet name="FISH_TOKEN_GENERATOR" sheetId="28" r:id="rId8"/>
-    <sheet name="FISH_TUNA" sheetId="37" r:id="rId9"/>
-    <sheet name="FISH_TUNA_ITEM" sheetId="35" r:id="rId10"/>
-    <sheet name="FISH_TUNA_ITEM_REFERENCE" sheetId="49" r:id="rId11"/>
-    <sheet name="FISH_TUNA_CUT" sheetId="39" r:id="rId12"/>
-    <sheet name="GOODS_RECEIPT" sheetId="19" r:id="rId13"/>
-    <sheet name="GOODS_ISSUE" sheetId="16" r:id="rId14"/>
+    <sheet name="FISH-CARD-GENERATOR" sheetId="27" r:id="rId6"/>
+    <sheet name="FISH-LABEL-GENERATOR" sheetId="34" r:id="rId7"/>
+    <sheet name="FISH-TOKEN-GENERATOR" sheetId="28" r:id="rId8"/>
+    <sheet name="FISH-TUNA" sheetId="37" r:id="rId9"/>
+    <sheet name="FISH-TUNA-ITEM" sheetId="35" r:id="rId10"/>
+    <sheet name="FISH-TUNA-ITEM-REFERENCE" sheetId="49" r:id="rId11"/>
+    <sheet name="FISH-TUNA-CUT" sheetId="39" r:id="rId12"/>
+    <sheet name="GOODS-RECEIPT" sheetId="19" r:id="rId13"/>
+    <sheet name="GOODS-ISSUE" sheetId="16" r:id="rId14"/>
     <sheet name="INVOICE" sheetId="20" r:id="rId15"/>
     <sheet name="INVENTORY" sheetId="25" r:id="rId16"/>
-    <sheet name="CUSTOMER_SALES" sheetId="26" r:id="rId17"/>
-    <sheet name="FSY-TUNA_FOOD" sheetId="31" r:id="rId18"/>
-    <sheet name="FSY-MALANG_STAFF" sheetId="29" r:id="rId19"/>
+    <sheet name="CUSTOMER-SALES" sheetId="26" r:id="rId17"/>
+    <sheet name="FSY-TUNA-FOOD" sheetId="31" r:id="rId18"/>
+    <sheet name="FSY-MALANG-STAFF" sheetId="29" r:id="rId19"/>
     <sheet name="FSY-VESSEL" sheetId="6" r:id="rId20"/>
     <sheet name="FSY-ROUTE" sheetId="7" r:id="rId21"/>
     <sheet name="FSY-TRIP" sheetId="8" r:id="rId22"/>
@@ -42,23 +42,21 @@
     <sheet name="FSY-PORT" sheetId="13" r:id="rId27"/>
     <sheet name="FSY-SCALE" sheetId="14" r:id="rId28"/>
     <sheet name="FSY-STORAGE" sheetId="15" r:id="rId29"/>
-    <sheet name="BATCH_NUMBER" sheetId="21" r:id="rId30"/>
+    <sheet name="BATCH-NUMBER" sheetId="21" r:id="rId30"/>
     <sheet name="CUSTOMER" sheetId="22" r:id="rId31"/>
     <sheet name="PRODUCT" sheetId="23" r:id="rId32"/>
     <sheet name="WAREHOUSE" sheetId="24" r:id="rId33"/>
     <sheet name="BANK" sheetId="30" r:id="rId34"/>
-    <sheet name="FSY-BUSINESS_UNIT" sheetId="32" r:id="rId35"/>
+    <sheet name="FSY-BUSINESS-UNIT" sheetId="32" r:id="rId35"/>
     <sheet name="FSY-CHEF" sheetId="33" r:id="rId36"/>
-    <sheet name="FISH_CARD" sheetId="40" r:id="rId37"/>
-    <sheet name="FISH_PART" sheetId="41" r:id="rId38"/>
-    <sheet name="FISH_STATUS" sheetId="42" r:id="rId39"/>
-    <sheet name="FISH_TOKEN" sheetId="43" r:id="rId40"/>
-    <sheet name="FSY_EMPLOYEE" sheetId="44" r:id="rId41"/>
-    <sheet name="FSY_TRIP" sheetId="45" r:id="rId42"/>
-    <sheet name="FSY_VESSEL" sheetId="46" r:id="rId43"/>
-    <sheet name="WEIGHT_LABEL" sheetId="47" r:id="rId44"/>
-    <sheet name="WEIGHT_TOKEN" sheetId="48" r:id="rId45"/>
-    <sheet name="FISH_ITEM_STATUS" sheetId="50" r:id="rId46"/>
+    <sheet name="FISH-CARD" sheetId="40" r:id="rId37"/>
+    <sheet name="FISH-PART" sheetId="41" r:id="rId38"/>
+    <sheet name="FISH-STATUS" sheetId="42" r:id="rId39"/>
+    <sheet name="FISH-TOKEN" sheetId="43" r:id="rId40"/>
+    <sheet name="FSY_VESSEL" sheetId="46" r:id="rId41"/>
+    <sheet name="WEIGHT-LABEL" sheetId="47" r:id="rId42"/>
+    <sheet name="WEIGHT-TOKEN" sheetId="48" r:id="rId43"/>
+    <sheet name="FISH-ITEM-STATUS" sheetId="50" r:id="rId44"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -70,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="284">
   <si>
     <t>TRANSACTION</t>
   </si>
@@ -303,9 +301,6 @@
     <t>Time Stamp</t>
   </si>
   <si>
-    <t>DATE_TIME</t>
-  </si>
-  <si>
     <t>longitude</t>
   </si>
   <si>
@@ -327,9 +322,6 @@
     <t>Capacity (GT)</t>
   </si>
   <si>
-    <t>#TEAM_MEMBER</t>
-  </si>
-  <si>
     <t>Team Member</t>
   </si>
   <si>
@@ -396,9 +388,6 @@
     <t>Customer #</t>
   </si>
   <si>
-    <t>GOODS_ISSUE</t>
-  </si>
-  <si>
     <t>WAREHOUSE</t>
   </si>
   <si>
@@ -417,12 +406,6 @@
     <t>PRODUCT</t>
   </si>
   <si>
-    <t>BATCH_NUMBER</t>
-  </si>
-  <si>
-    <t>GOODS_RECEIPT</t>
-  </si>
-  <si>
     <t>quantityReceipt</t>
   </si>
   <si>
@@ -486,9 +469,6 @@
     <t>02. Customer Sales</t>
   </si>
   <si>
-    <t>CUSTOMER_SALES</t>
-  </si>
-  <si>
     <t>SHORT_STRING</t>
   </si>
   <si>
@@ -513,45 +493,27 @@
     <t>Fish Token</t>
   </si>
   <si>
-    <t>#FISH_CARD</t>
-  </si>
-  <si>
     <t>01. Fish Card Generator</t>
   </si>
   <si>
-    <t>FISH_CARD_GENERATOR</t>
-  </si>
-  <si>
     <t>Prefix</t>
   </si>
   <si>
     <t>INTEGER</t>
   </si>
   <si>
-    <t>FISH_TOKEN_GENERATOR</t>
-  </si>
-  <si>
     <t>02. Fish Token Generator</t>
   </si>
   <si>
-    <t>#FISH_WEIGHT</t>
-  </si>
-  <si>
     <t>Weight</t>
   </si>
   <si>
-    <t>#FISH_TOKEN</t>
-  </si>
-  <si>
     <t>fishWeight</t>
   </si>
   <si>
     <t>Fish Weight</t>
   </si>
   <si>
-    <t>FSY-MALANG_STAFF</t>
-  </si>
-  <si>
     <t>Role</t>
   </si>
   <si>
@@ -615,9 +577,6 @@
     <t>90. Project/06. Project Malang</t>
   </si>
   <si>
-    <t>FSY-TUNA_FOOD</t>
-  </si>
-  <si>
     <t>chef</t>
   </si>
   <si>
@@ -633,9 +592,6 @@
     <t>SBU #</t>
   </si>
   <si>
-    <t>FSY-BUSINESS_UNIT</t>
-  </si>
-  <si>
     <t>02. Tuna Food</t>
   </si>
   <si>
@@ -669,9 +625,6 @@
     <t>address</t>
   </si>
   <si>
-    <t>LONG_STRING</t>
-  </si>
-  <si>
     <t>website</t>
   </si>
   <si>
@@ -738,9 +691,6 @@
     <t>Fish Parent Label</t>
   </si>
   <si>
-    <t>FISH_LABEL_GENERATOR</t>
-  </si>
-  <si>
     <t>03. Fish Label Generator</t>
   </si>
   <si>
@@ -780,42 +730,27 @@
     <t>Date Caught</t>
   </si>
   <si>
-    <t>FISH_TUNA</t>
-  </si>
-  <si>
     <t>01. Tuna</t>
   </si>
   <si>
     <t>Fish Card #</t>
   </si>
   <si>
-    <t>FISH_CARD</t>
-  </si>
-  <si>
     <t>Fish Token #</t>
   </si>
   <si>
-    <t>FISH_TOKEN</t>
-  </si>
-  <si>
     <t>weightLabel</t>
   </si>
   <si>
     <t>Weight Label #</t>
   </si>
   <si>
-    <t>WEIGHT_LABEL</t>
-  </si>
-  <si>
     <t>weightToken</t>
   </si>
   <si>
     <t>Weight Token #</t>
   </si>
   <si>
-    <t>WEIGHT_TOKEN</t>
-  </si>
-  <si>
     <t>Weight Actual (KG)</t>
   </si>
   <si>
@@ -825,15 +760,6 @@
     <t>Fish Trip #</t>
   </si>
   <si>
-    <t>FSY_TRIP</t>
-  </si>
-  <si>
-    <t>FSY_VESSEL</t>
-  </si>
-  <si>
-    <t>FSY_EMPLOYEE</t>
-  </si>
-  <si>
     <t>DATE</t>
   </si>
   <si>
@@ -843,9 +769,6 @@
     <t>Fish Tuna #</t>
   </si>
   <si>
-    <t>FISH_TUNA_ITEM</t>
-  </si>
-  <si>
     <t>02. Fish/01. Tuna</t>
   </si>
   <si>
@@ -864,24 +787,15 @@
     <t>Fish Part</t>
   </si>
   <si>
-    <t>FISH_PART</t>
-  </si>
-  <si>
     <t>weight</t>
   </si>
   <si>
     <t>fishItemParent</t>
   </si>
   <si>
-    <t>FISH_STATUS</t>
-  </si>
-  <si>
     <t>Fish Item Parent #</t>
   </si>
   <si>
-    <t>#FISH_PART</t>
-  </si>
-  <si>
     <t>weightChildren</t>
   </si>
   <si>
@@ -903,24 +817,15 @@
     <t>dateRelease</t>
   </si>
   <si>
-    <t>FISH_TUNA_CUT</t>
-  </si>
-  <si>
     <t>fishItemStatus</t>
   </si>
   <si>
     <t>Fish Item Status #</t>
   </si>
   <si>
-    <t>FISH_ITEM_STATUS</t>
-  </si>
-  <si>
     <t>02. Tuna Item</t>
   </si>
   <si>
-    <t>FISH_TUNA_ITEM_REFERENCE</t>
-  </si>
-  <si>
     <t>03. Tuna Item Reference</t>
   </si>
   <si>
@@ -931,6 +836,90 @@
   </si>
   <si>
     <t>Length</t>
+  </si>
+  <si>
+    <t>FISH-CARD-GENERATOR</t>
+  </si>
+  <si>
+    <t>#FISH-CARD</t>
+  </si>
+  <si>
+    <t>FISH-LABEL-GENERATOR</t>
+  </si>
+  <si>
+    <t>#FISH-TOKEN</t>
+  </si>
+  <si>
+    <t>FISH-TOKEN-GENERATOR</t>
+  </si>
+  <si>
+    <t>#FISH-WEIGHT</t>
+  </si>
+  <si>
+    <t>FISH-TUNA</t>
+  </si>
+  <si>
+    <t>FISH-CARD</t>
+  </si>
+  <si>
+    <t>FISH-TOKEN</t>
+  </si>
+  <si>
+    <t>WEIGHT-LABEL</t>
+  </si>
+  <si>
+    <t>WEIGHT-TOKEN</t>
+  </si>
+  <si>
+    <t>#FISH-PART</t>
+  </si>
+  <si>
+    <t>FISH-PART</t>
+  </si>
+  <si>
+    <t>FISH-TUNA-ITEM</t>
+  </si>
+  <si>
+    <t>FISH-TUNA-ITEM-REFERENCE</t>
+  </si>
+  <si>
+    <t>FISH-ITEM-STATUS</t>
+  </si>
+  <si>
+    <t>DATE-TIME</t>
+  </si>
+  <si>
+    <t>FISH-TUNA-CUT</t>
+  </si>
+  <si>
+    <t>GOODS-RECEIPT</t>
+  </si>
+  <si>
+    <t>BATCH-NUMBER</t>
+  </si>
+  <si>
+    <t>GOODS-ISSUE</t>
+  </si>
+  <si>
+    <t>CUSTOMER-SALES</t>
+  </si>
+  <si>
+    <t>FSY-TUNA-FOOD</t>
+  </si>
+  <si>
+    <t>FSY-MALANG-STAFF</t>
+  </si>
+  <si>
+    <t>FSY-BUSINESS-UNIT</t>
+  </si>
+  <si>
+    <t>#TEAM-MEMBER</t>
+  </si>
+  <si>
+    <t>LONG-STRING</t>
+  </si>
+  <si>
+    <t>FISH-STATUS</t>
   </si>
 </sst>
 </file>
@@ -1348,7 +1337,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1372,7 +1361,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
@@ -1481,76 +1470,76 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>281</v>
+        <v>251</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>236</v>
+        <v>262</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>266</v>
+        <v>240</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>278</v>
+        <v>249</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>279</v>
+        <v>250</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>272</v>
+        <v>244</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>2</v>
@@ -1561,10 +1550,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>270</v>
+        <v>242</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>273</v>
+        <v>245</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>2</v>
@@ -1575,10 +1564,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>274</v>
+        <v>246</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>2</v>
@@ -1589,13 +1578,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>276</v>
+        <v>248</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>77</v>
+        <v>272</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -1631,34 +1620,34 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>283</v>
+        <v>252</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>236</v>
+        <v>262</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -1693,44 +1682,44 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>284</v>
+        <v>253</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>266</v>
+        <v>240</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>272</v>
+        <v>244</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>2</v>
@@ -1741,10 +1730,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>270</v>
+        <v>242</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>273</v>
+        <v>245</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>2</v>
@@ -1755,10 +1744,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>274</v>
+        <v>246</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>2</v>
@@ -1769,10 +1758,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1781,26 +1770,26 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>265</v>
+        <v>239</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>271</v>
+        <v>243</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>2</v>
@@ -1841,50 +1830,50 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>116</v>
+        <v>274</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>116</v>
+        <v>274</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -1903,7 +1892,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
@@ -1912,30 +1901,30 @@
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>115</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1948,7 +1937,7 @@
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I19" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1978,50 +1967,50 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>276</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>108</v>
+        <v>276</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -2040,7 +2029,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
@@ -2049,30 +2038,30 @@
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>115</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -2110,34 +2099,34 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -2156,7 +2145,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>4</v>
@@ -2165,30 +2154,30 @@
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>115</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -2196,10 +2185,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -2207,10 +2196,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -2246,25 +2235,25 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
@@ -2273,46 +2262,46 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>115</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -2348,25 +2337,25 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>277</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
+        <v>277</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
@@ -2375,46 +2364,46 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>115</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -2435,7 +2424,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="H1:I1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2445,79 +2434,79 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>181</v>
+        <v>278</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>159</v>
+        <v>279</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>187</v>
+        <v>280</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>159</v>
+        <v>279</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="2"/>
@@ -2525,13 +2514,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="2"/>
@@ -2539,13 +2528,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2578,19 +2567,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>159</v>
+        <v>279</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>159</v>
+        <v>279</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -2599,10 +2588,10 @@
         <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -2610,13 +2599,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -2624,13 +2613,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="2"/>
@@ -2638,13 +2627,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="2"/>
@@ -2652,29 +2641,29 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2682,13 +2671,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2733,7 +2722,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>33</v>
@@ -2773,7 +2762,7 @@
         <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2793,7 +2782,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2813,7 +2802,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2846,7 +2835,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F7" s="3"/>
     </row>
@@ -2866,13 +2855,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
@@ -2943,13 +2932,13 @@
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>13</v>
@@ -2958,10 +2947,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -2985,7 +2974,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3008,7 +2997,7 @@
         <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>12</v>
@@ -3079,16 +3068,16 @@
         <v>76</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>77</v>
+        <v>272</v>
       </c>
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" t="s">
         <v>78</v>
-      </c>
-      <c r="B6" t="s">
-        <v>79</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -3097,10 +3086,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" t="s">
         <v>80</v>
-      </c>
-      <c r="B7" t="s">
-        <v>81</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -3121,9 +3110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566FD6AA-D77E-B74F-9E88-1F6BFA48CD94}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3146,7 +3133,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>12</v>
@@ -3187,10 +3174,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>85</v>
+        <v>281</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -3216,7 +3203,7 @@
         <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -3256,7 +3243,7 @@
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3285,7 +3272,7 @@
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3314,7 +3301,7 @@
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3343,7 +3330,7 @@
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3372,7 +3359,7 @@
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3401,7 +3388,7 @@
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3430,7 +3417,7 @@
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3466,7 +3453,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>41</v>
@@ -3506,7 +3493,7 @@
         <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -3526,7 +3513,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -3546,7 +3533,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -3595,10 +3582,10 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -3620,13 +3607,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
@@ -3680,16 +3667,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>275</v>
       </c>
       <c r="B1" t="s">
-        <v>115</v>
+        <v>275</v>
       </c>
       <c r="C1" t="s">
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3709,16 +3696,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C1" t="s">
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3738,16 +3725,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C1" t="s">
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3767,16 +3754,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3796,16 +3783,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="B1" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C1" t="s">
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3831,71 +3818,71 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>187</v>
+        <v>280</v>
       </c>
       <c r="B1" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="C1" t="s">
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="C2" t="s">
-        <v>199</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="B3" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="B4" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="C4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="B5" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="C5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="B6" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="C6" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -3915,49 +3902,49 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="B1" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C1" t="s">
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B2" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="C2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="C3" t="s">
-        <v>199</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="C4" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -3977,16 +3964,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="B1" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="C1" t="s">
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -4006,16 +3993,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B1" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="C1" t="s">
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -4035,16 +4022,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>267</v>
+        <v>283</v>
       </c>
       <c r="B1" t="s">
-        <v>267</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -4081,7 +4068,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>52</v>
@@ -4090,7 +4077,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>51</v>
@@ -4121,7 +4108,7 @@
         <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -4141,7 +4128,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -4161,7 +4148,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -4181,7 +4168,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -4210,10 +4197,10 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -4235,13 +4222,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
@@ -4295,16 +4282,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>241</v>
+        <v>264</v>
       </c>
       <c r="B1" t="s">
-        <v>241</v>
+        <v>264</v>
       </c>
       <c r="C1" t="s">
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -4313,64 +4300,6 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B1" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B1" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -4382,16 +4311,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>252</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>252</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -4399,7 +4328,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -4411,16 +4340,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>244</v>
+        <v>265</v>
       </c>
       <c r="B1" t="s">
-        <v>244</v>
+        <v>265</v>
       </c>
       <c r="C1" t="s">
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -4428,7 +4357,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -4440,16 +4369,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>247</v>
+        <v>266</v>
       </c>
       <c r="B1" t="s">
-        <v>247</v>
+        <v>266</v>
       </c>
       <c r="C1" t="s">
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -4457,28 +4386,28 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="B1" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="C1" t="s">
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -4517,7 +4446,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>54</v>
@@ -4557,7 +4486,7 @@
         <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -4577,7 +4506,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -4597,7 +4526,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -4646,10 +4575,10 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -4671,13 +4600,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
@@ -4721,10 +4650,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4218953-49A7-7A4A-B095-3E11504A1649}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4741,31 +4670,31 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>149</v>
+        <v>256</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>149</v>
+        <v>256</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -4773,13 +4702,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -4787,10 +4716,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>147</v>
+        <v>257</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -4799,13 +4728,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -4813,13 +4742,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -4828,11 +4757,6 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I18" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -4844,7 +4768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737A8CBA-46B9-4E45-AC34-E9F3DB9DC043}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -4856,31 +4780,31 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -4888,13 +4812,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -4902,13 +4826,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -4916,13 +4840,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -4930,13 +4854,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -4944,13 +4868,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -4958,13 +4882,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -4972,10 +4896,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>156</v>
+        <v>259</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -4984,13 +4908,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -4998,13 +4922,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -5012,13 +4936,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>286</v>
+        <v>255</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -5056,31 +4980,31 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>152</v>
+        <v>260</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>152</v>
+        <v>260</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -5088,10 +5012,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>154</v>
+        <v>261</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -5100,13 +5024,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -5114,10 +5038,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>156</v>
+        <v>259</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -5126,13 +5050,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -5140,13 +5064,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -5159,7 +5083,7 @@
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I19" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -5172,7 +5096,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="H1:I1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5186,66 +5110,66 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>236</v>
+        <v>262</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>236</v>
+        <v>262</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>241</v>
+        <v>264</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>251</v>
+        <v>12</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -5261,7 +5185,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>252</v>
+        <v>13</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -5277,20 +5201,20 @@
         <v>1</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>253</v>
+        <v>70</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -5298,42 +5222,42 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>244</v>
+        <v>265</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>247</v>
+        <v>266</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>2</v>
@@ -5344,10 +5268,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>2</v>
@@ -5358,10 +5282,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -5370,26 +5294,26 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>265</v>
+        <v>239</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>271</v>
+        <v>243</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
From bjo-sea01 fix vessel 2023-12-01.005607
</commit_message>
<xml_diff>
--- a/config/config/data-structure.SEA01.xlsx
+++ b/config/config/data-structure.SEA01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/Documents/docker/data/client/ysh/client/bjo-sea01/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3CF358-A5C4-F541-A137-D26449287D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EAEABF-5963-F040-B4E1-7974AE63F6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="6160" windowWidth="28360" windowHeight="17620" firstSheet="33" activeTab="43" xr2:uid="{A25778A6-52F4-354B-B7EA-075EA69C9E88}"/>
+    <workbookView xWindow="2040" yWindow="6160" windowWidth="28360" windowHeight="17620" firstSheet="25" activeTab="35" xr2:uid="{A25778A6-52F4-354B-B7EA-075EA69C9E88}"/>
   </bookViews>
   <sheets>
     <sheet name="FSY-01-UNLOADING" sheetId="1" r:id="rId1"/>
@@ -53,10 +53,9 @@
     <sheet name="FISH-PART" sheetId="41" r:id="rId38"/>
     <sheet name="FISH-STATUS" sheetId="42" r:id="rId39"/>
     <sheet name="FISH-TOKEN" sheetId="43" r:id="rId40"/>
-    <sheet name="FSY_VESSEL" sheetId="46" r:id="rId41"/>
-    <sheet name="WEIGHT-LABEL" sheetId="47" r:id="rId42"/>
-    <sheet name="WEIGHT-TOKEN" sheetId="48" r:id="rId43"/>
-    <sheet name="FISH-ITEM-STATUS" sheetId="50" r:id="rId44"/>
+    <sheet name="WEIGHT-LABEL" sheetId="47" r:id="rId41"/>
+    <sheet name="WEIGHT-TOKEN" sheetId="48" r:id="rId42"/>
+    <sheet name="FISH-ITEM-STATUS" sheetId="50" r:id="rId43"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -68,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="284">
   <si>
     <t>TRANSACTION</t>
   </si>
@@ -2424,7 +2423,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3894,11 +3893,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -4300,35 +4305,6 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -4357,7 +4333,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -4386,11 +4362,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
From bjo-sea01 fix vessel 2023-12-01.005937
</commit_message>
<xml_diff>
--- a/config/config/data-structure.SEA01.xlsx
+++ b/config/config/data-structure.SEA01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/Documents/docker/data/client/ysh/client/bjo-sea01/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EAEABF-5963-F040-B4E1-7974AE63F6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AC588B-5F9D-E748-B5DA-A877686467F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="6160" windowWidth="28360" windowHeight="17620" firstSheet="25" activeTab="35" xr2:uid="{A25778A6-52F4-354B-B7EA-075EA69C9E88}"/>
   </bookViews>
@@ -885,9 +885,6 @@
     <t>FISH-ITEM-STATUS</t>
   </si>
   <si>
-    <t>DATE-TIME</t>
-  </si>
-  <si>
     <t>FISH-TUNA-CUT</t>
   </si>
   <si>
@@ -919,6 +916,9 @@
   </si>
   <si>
     <t>FISH-STATUS</t>
+  </si>
+  <si>
+    <t>DATE_TIME</t>
   </si>
 </sst>
 </file>
@@ -1583,7 +1583,7 @@
         <v>247</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -1681,7 +1681,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>253</v>
@@ -1693,7 +1693,7 @@
         <v>233</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -1829,7 +1829,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>123</v>
@@ -1841,7 +1841,7 @@
         <v>165</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -1915,7 +1915,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1966,7 +1966,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>121</v>
@@ -1978,7 +1978,7 @@
         <v>165</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -2052,7 +2052,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2168,7 +2168,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2292,7 +2292,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2336,7 +2336,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>132</v>
@@ -2348,7 +2348,7 @@
         <v>166</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -2394,7 +2394,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2433,7 +2433,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>174</v>
@@ -2445,7 +2445,7 @@
         <v>199</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -2476,7 +2476,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -2492,7 +2492,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -2566,7 +2566,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>167</v>
@@ -2578,7 +2578,7 @@
         <v>168</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -3067,7 +3067,7 @@
         <v>76</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -3173,7 +3173,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>84</v>
@@ -3666,10 +3666,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C1" t="s">
         <v>74</v>
@@ -3817,7 +3817,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B1" t="s">
         <v>182</v>
@@ -3837,7 +3837,7 @@
         <v>183</v>
       </c>
       <c r="C2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3894,7 +3894,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="K19" activeCellId="1" sqref="D6 K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3938,7 +3938,7 @@
         <v>192</v>
       </c>
       <c r="C3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4027,10 +4027,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C1" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
From bjo-sea01 fix long- 2023-12-01.010101
</commit_message>
<xml_diff>
--- a/config/config/data-structure.SEA01.xlsx
+++ b/config/config/data-structure.SEA01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/Documents/docker/data/client/ysh/client/bjo-sea01/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AC588B-5F9D-E748-B5DA-A877686467F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694B3EB5-5A88-0D40-B0C5-00E305EF861F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="6160" windowWidth="28360" windowHeight="17620" firstSheet="25" activeTab="35" xr2:uid="{A25778A6-52F4-354B-B7EA-075EA69C9E88}"/>
   </bookViews>
@@ -912,13 +912,13 @@
     <t>#TEAM-MEMBER</t>
   </si>
   <si>
-    <t>LONG-STRING</t>
-  </si>
-  <si>
     <t>FISH-STATUS</t>
   </si>
   <si>
     <t>DATE_TIME</t>
+  </si>
+  <si>
+    <t>LONG_STRING</t>
   </si>
 </sst>
 </file>
@@ -1583,7 +1583,7 @@
         <v>247</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -3067,7 +3067,7 @@
         <v>76</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -3837,7 +3837,7 @@
         <v>183</v>
       </c>
       <c r="C2" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3894,7 +3894,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" activeCellId="1" sqref="D6 K19"/>
+      <selection activeCell="K19" activeCellId="1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3938,7 +3938,7 @@
         <v>192</v>
       </c>
       <c r="C3" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4027,10 +4027,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C1" t="s">
         <v>74</v>

</xml_diff>